<commit_message>
added csv files for recreating own figure (hw3 pt1) and a png of the original figure
</commit_message>
<xml_diff>
--- a/hw3/figData.xlsx
+++ b/hw3/figData.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
   <si>
     <t>NegCueSD-NegCueSR</t>
   </si>
@@ -28,6 +28,24 @@
   </si>
   <si>
     <t>AmbCueSD-AmbCueSR</t>
+  </si>
+  <si>
+    <t>NegCueSD</t>
+  </si>
+  <si>
+    <t>NeuCueSD</t>
+  </si>
+  <si>
+    <t>AmbCueSD</t>
+  </si>
+  <si>
+    <t>NegCueSR</t>
+  </si>
+  <si>
+    <t>NeuCueSR</t>
+  </si>
+  <si>
+    <t>AmbCueSR</t>
   </si>
 </sst>
 </file>
@@ -396,15 +414,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C19"/>
+  <dimension ref="A1:I19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+      <selection activeCell="D1" sqref="D1:I19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:9">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -414,8 +432,26 @@
       <c r="C1" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="2" spans="1:3">
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9">
       <c r="A2">
         <v>0.90849899999999995</v>
       </c>
@@ -425,8 +461,26 @@
       <c r="C2">
         <v>-0.60556699999999997</v>
       </c>
-    </row>
-    <row r="3" spans="1:3">
+      <c r="D2">
+        <v>7.2172E-2</v>
+      </c>
+      <c r="E2">
+        <v>-1.04497</v>
+      </c>
+      <c r="F2">
+        <v>-0.63670300000000002</v>
+      </c>
+      <c r="G2">
+        <v>-0.83632700000000004</v>
+      </c>
+      <c r="H2">
+        <v>-0.15805900000000001</v>
+      </c>
+      <c r="I2">
+        <v>-3.1136299999999999E-2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9">
       <c r="A3">
         <v>0.334592</v>
       </c>
@@ -436,8 +490,26 @@
       <c r="C3">
         <v>-0.573407</v>
       </c>
-    </row>
-    <row r="4" spans="1:3">
+      <c r="D3">
+        <v>-0.35364800000000002</v>
+      </c>
+      <c r="E3">
+        <v>-1.3544400000000001</v>
+      </c>
+      <c r="F3">
+        <v>-0.51698</v>
+      </c>
+      <c r="G3">
+        <v>-0.68823999999999996</v>
+      </c>
+      <c r="H3">
+        <v>-0.78481800000000002</v>
+      </c>
+      <c r="I3">
+        <v>5.6426700000000003E-2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9">
       <c r="A4">
         <v>0.14479300000000001</v>
       </c>
@@ -447,8 +519,26 @@
       <c r="C4">
         <v>0.43743399999999999</v>
       </c>
-    </row>
-    <row r="5" spans="1:3">
+      <c r="D4">
+        <v>-0.25640099999999999</v>
+      </c>
+      <c r="E4">
+        <v>-0.85672199999999998</v>
+      </c>
+      <c r="F4">
+        <v>0.102033</v>
+      </c>
+      <c r="G4">
+        <v>-0.401194</v>
+      </c>
+      <c r="H4">
+        <v>-2.13203E-2</v>
+      </c>
+      <c r="I4">
+        <v>-0.335401</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9">
       <c r="A5">
         <v>0.87887199999999999</v>
       </c>
@@ -458,8 +548,26 @@
       <c r="C5">
         <v>1.37279</v>
       </c>
-    </row>
-    <row r="6" spans="1:3">
+      <c r="D5">
+        <v>4.9569099999999998E-2</v>
+      </c>
+      <c r="E5">
+        <v>-0.41718899999999998</v>
+      </c>
+      <c r="F5">
+        <v>0.117841</v>
+      </c>
+      <c r="G5">
+        <v>-0.82930300000000001</v>
+      </c>
+      <c r="H5">
+        <v>-0.79979999999999996</v>
+      </c>
+      <c r="I5">
+        <v>-1.25495</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9">
       <c r="A6">
         <v>0.13433100000000001</v>
       </c>
@@ -469,8 +577,26 @@
       <c r="C6">
         <v>0.58831999999999995</v>
       </c>
-    </row>
-    <row r="7" spans="1:3">
+      <c r="D6">
+        <v>0.16500500000000001</v>
+      </c>
+      <c r="E6">
+        <v>1.75244</v>
+      </c>
+      <c r="F6">
+        <v>0.89788000000000001</v>
+      </c>
+      <c r="G6">
+        <v>3.0674199999999999E-2</v>
+      </c>
+      <c r="H6">
+        <v>-0.50628499999999999</v>
+      </c>
+      <c r="I6">
+        <v>0.30956</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9">
       <c r="A7">
         <v>1.5831299999999999</v>
       </c>
@@ -480,8 +606,26 @@
       <c r="C7">
         <v>1.01936</v>
       </c>
-    </row>
-    <row r="8" spans="1:3">
+      <c r="D7">
+        <v>-3.1559499999999998E-3</v>
+      </c>
+      <c r="E7">
+        <v>0.51102199999999998</v>
+      </c>
+      <c r="F7">
+        <v>-0.122243</v>
+      </c>
+      <c r="G7">
+        <v>-1.58629</v>
+      </c>
+      <c r="H7">
+        <v>-1.40585</v>
+      </c>
+      <c r="I7">
+        <v>-1.14161</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9">
       <c r="A8">
         <v>2.0702600000000002</v>
       </c>
@@ -491,8 +635,26 @@
       <c r="C8">
         <v>0.75309999999999999</v>
       </c>
-    </row>
-    <row r="9" spans="1:3">
+      <c r="D8">
+        <v>0.60167300000000001</v>
+      </c>
+      <c r="E8">
+        <v>9.9601300000000004E-2</v>
+      </c>
+      <c r="F8">
+        <v>-0.33981499999999998</v>
+      </c>
+      <c r="G8">
+        <v>-1.46858</v>
+      </c>
+      <c r="H8">
+        <v>-1.05149</v>
+      </c>
+      <c r="I8">
+        <v>-1.09291</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9">
       <c r="A9">
         <v>1.3731100000000001</v>
       </c>
@@ -502,8 +664,26 @@
       <c r="C9">
         <v>-0.67025800000000002</v>
       </c>
-    </row>
-    <row r="10" spans="1:3">
+      <c r="D9">
+        <v>-1.53888</v>
+      </c>
+      <c r="E9">
+        <v>-1.3232900000000001</v>
+      </c>
+      <c r="F9">
+        <v>-1.2446999999999999</v>
+      </c>
+      <c r="G9">
+        <v>-2.9119799999999998</v>
+      </c>
+      <c r="H9">
+        <v>-2.1977099999999998</v>
+      </c>
+      <c r="I9">
+        <v>-0.57444499999999998</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9">
       <c r="A10">
         <v>-4.0479899999999999E-2</v>
       </c>
@@ -513,8 +693,26 @@
       <c r="C10">
         <v>-0.58687500000000004</v>
       </c>
-    </row>
-    <row r="11" spans="1:3">
+      <c r="D10">
+        <v>-0.63909199999999999</v>
+      </c>
+      <c r="E10">
+        <v>-1.9362999999999999</v>
+      </c>
+      <c r="F10">
+        <v>-1.6834499999999999</v>
+      </c>
+      <c r="G10">
+        <v>-0.59861200000000003</v>
+      </c>
+      <c r="H10">
+        <v>-0.91163499999999997</v>
+      </c>
+      <c r="I10">
+        <v>-1.09657</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9">
       <c r="A11">
         <v>1.1680900000000001</v>
       </c>
@@ -524,8 +722,26 @@
       <c r="C11">
         <v>-0.35735299999999998</v>
       </c>
-    </row>
-    <row r="12" spans="1:3">
+      <c r="D11">
+        <v>0.305705</v>
+      </c>
+      <c r="E11">
+        <v>0.44490200000000002</v>
+      </c>
+      <c r="F11">
+        <v>-0.53134099999999995</v>
+      </c>
+      <c r="G11">
+        <v>-0.86238999999999999</v>
+      </c>
+      <c r="H11">
+        <v>-1.2040200000000001</v>
+      </c>
+      <c r="I11">
+        <v>-0.173988</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9">
       <c r="A12">
         <v>0.83308800000000005</v>
       </c>
@@ -535,8 +751,26 @@
       <c r="C12">
         <v>9.5179399999999997E-2</v>
       </c>
-    </row>
-    <row r="13" spans="1:3">
+      <c r="D12">
+        <v>0.55860399999999999</v>
+      </c>
+      <c r="E12">
+        <v>-0.138457</v>
+      </c>
+      <c r="F12">
+        <v>-7.8146900000000005E-2</v>
+      </c>
+      <c r="G12">
+        <v>-0.27448400000000001</v>
+      </c>
+      <c r="H12">
+        <v>-0.75865899999999997</v>
+      </c>
+      <c r="I12">
+        <v>-0.17332600000000001</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9">
       <c r="A13">
         <v>4.3210499999999999E-2</v>
       </c>
@@ -546,8 +780,26 @@
       <c r="C13">
         <v>-0.58355000000000001</v>
       </c>
-    </row>
-    <row r="14" spans="1:3">
+      <c r="D13">
+        <v>-1.55924</v>
+      </c>
+      <c r="E13">
+        <v>-1.77223</v>
+      </c>
+      <c r="F13">
+        <v>-1.4180600000000001</v>
+      </c>
+      <c r="G13">
+        <v>-1.6024499999999999</v>
+      </c>
+      <c r="H13">
+        <v>-1.6919999999999999</v>
+      </c>
+      <c r="I13">
+        <v>-0.83450500000000005</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9">
       <c r="A14">
         <v>-0.99458599999999997</v>
       </c>
@@ -557,8 +809,26 @@
       <c r="C14">
         <v>0.433112</v>
       </c>
-    </row>
-    <row r="15" spans="1:3">
+      <c r="D14">
+        <v>-0.20743200000000001</v>
+      </c>
+      <c r="E14">
+        <v>0.44318600000000002</v>
+      </c>
+      <c r="F14">
+        <v>0.166934</v>
+      </c>
+      <c r="G14">
+        <v>0.78715400000000002</v>
+      </c>
+      <c r="H14">
+        <v>-0.36180600000000002</v>
+      </c>
+      <c r="I14">
+        <v>-0.266177</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9">
       <c r="A15">
         <v>1.51376</v>
       </c>
@@ -568,8 +838,26 @@
       <c r="C15">
         <v>-3.00945E-2</v>
       </c>
-    </row>
-    <row r="16" spans="1:3">
+      <c r="D15">
+        <v>0.40691899999999998</v>
+      </c>
+      <c r="E15">
+        <v>-0.64551800000000004</v>
+      </c>
+      <c r="F15">
+        <v>-0.90568599999999999</v>
+      </c>
+      <c r="G15">
+        <v>-1.10684</v>
+      </c>
+      <c r="H15">
+        <v>-1.3048299999999999</v>
+      </c>
+      <c r="I15">
+        <v>-0.87559200000000004</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9">
       <c r="A16">
         <v>-2.17456E-2</v>
       </c>
@@ -579,8 +867,26 @@
       <c r="C16">
         <v>0.25034000000000001</v>
       </c>
-    </row>
-    <row r="17" spans="1:3">
+      <c r="D16">
+        <v>-0.351634</v>
+      </c>
+      <c r="E16">
+        <v>0.16514400000000001</v>
+      </c>
+      <c r="F16">
+        <v>-0.21924399999999999</v>
+      </c>
+      <c r="G16">
+        <v>-0.32988899999999999</v>
+      </c>
+      <c r="H16">
+        <v>-0.93241099999999999</v>
+      </c>
+      <c r="I16">
+        <v>-0.469584</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9">
       <c r="A17">
         <v>1.5870500000000001</v>
       </c>
@@ -590,8 +896,26 @@
       <c r="C17">
         <v>0.86927500000000002</v>
       </c>
-    </row>
-    <row r="18" spans="1:3">
+      <c r="D17">
+        <v>0.993676</v>
+      </c>
+      <c r="E17">
+        <v>0.335478</v>
+      </c>
+      <c r="F17">
+        <v>0.41409499999999999</v>
+      </c>
+      <c r="G17">
+        <v>-0.59337799999999996</v>
+      </c>
+      <c r="H17">
+        <v>-0.52339100000000005</v>
+      </c>
+      <c r="I17">
+        <v>-0.45517999999999997</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9">
       <c r="A18">
         <v>1.5646800000000001</v>
       </c>
@@ -601,8 +925,26 @@
       <c r="C18">
         <v>-0.18831300000000001</v>
       </c>
-    </row>
-    <row r="19" spans="1:3">
+      <c r="D18">
+        <v>0.43606400000000001</v>
+      </c>
+      <c r="E18">
+        <v>-0.102812</v>
+      </c>
+      <c r="F18">
+        <v>-0.41386699999999998</v>
+      </c>
+      <c r="G18">
+        <v>-1.12862</v>
+      </c>
+      <c r="H18">
+        <v>-0.93374199999999996</v>
+      </c>
+      <c r="I18">
+        <v>-0.225554</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9">
       <c r="A19">
         <v>0.79413299999999998</v>
       </c>
@@ -611,6 +953,24 @@
       </c>
       <c r="C19">
         <v>0.47291</v>
+      </c>
+      <c r="D19">
+        <v>-7.2258799999999998E-2</v>
+      </c>
+      <c r="E19">
+        <v>0.35768800000000001</v>
+      </c>
+      <c r="F19">
+        <v>-0.90640900000000002</v>
+      </c>
+      <c r="G19">
+        <v>-0.86639200000000005</v>
+      </c>
+      <c r="H19">
+        <v>-0.61735099999999998</v>
+      </c>
+      <c r="I19">
+        <v>-1.3793200000000001</v>
       </c>
     </row>
   </sheetData>

</xml_diff>